<commit_message>
- deleted filled out fields
</commit_message>
<xml_diff>
--- a/inst/quality/PerformanceIndicators.xlsx
+++ b/inst/quality/PerformanceIndicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Statistical matters\ProjectSetup\prodigenrCCMS\inst\quality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Statistical matters\ProjectSetup\prodigenrCCMS\inst\quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Performance Indicators for CCMS</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>Number of patients planned</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Finished</t>
   </si>
   <si>
     <t>Final number of patients in analysis</t>
@@ -938,12 +932,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -987,6 +975,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,7 +1340,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,619 +1360,613 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="27" t="s">
+      <c r="P2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="S2" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="19"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="17"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="11"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="11"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="9"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="11"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="9"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="11"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="9"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="11"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="9"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="9"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="11"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="9"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="31"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="29"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="35"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="33"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="9"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="9"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="11"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="9"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="11"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="9"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="11"/>
+      <c r="A18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="9"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="9"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="9"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="11"/>
+      <c r="A21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="9"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="11"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="9"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="11"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="9"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="11"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="9"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="11"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="9"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="12"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2065,7 +2053,7 @@
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="47" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2073,7 +2061,7 @@
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">

</xml_diff>